<commit_message>
added a Slave node Code
</commit_message>
<xml_diff>
--- a/Testprotokoll.xlsx
+++ b/Testprotokoll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loris\Desktop\GitHub\BLJ2022_uek216_lift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BAEE63-38D4-44DB-BBBF-97586E0EC388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0F3293-A92D-4936-B1C7-81075A983D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15075" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -554,13 +554,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="193" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
     <col min="4" max="5" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>